<commit_message>
added more volumes filtered
</commit_message>
<xml_diff>
--- a/data/permanent mount index.xlsx
+++ b/data/permanent mount index.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/fournier_sophie_epa_gov/Documents/Lab/Fluorometer Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SFOURNIE\Git\fluoroproj\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="190" documentId="13_ncr:1_{B7069C09-D807-41F2-BDAC-B0AEA3B90F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8BC9C26-FE34-404A-B330-5E8FCFCC5037}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{437C1489-2E86-4FDA-8BB3-5F8BCCBBB550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9E43A6A2-D3AC-4401-99CB-597ABF4CC040}"/>
   </bookViews>
@@ -465,8 +465,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F7CEBF0-92B3-43F1-B1F9-2D4CC5B9898C}">
   <dimension ref="A1:H145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H80" sqref="H80"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H116" sqref="H116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2512,6 +2513,9 @@
       <c r="G86">
         <v>1</v>
       </c>
+      <c r="H86" s="1">
+        <v>10</v>
+      </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87">
@@ -2532,6 +2536,9 @@
       <c r="G87">
         <v>2</v>
       </c>
+      <c r="H87" s="1">
+        <v>10</v>
+      </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88">
@@ -2552,6 +2559,9 @@
       <c r="G88">
         <v>3</v>
       </c>
+      <c r="H88" s="1">
+        <v>10</v>
+      </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89">
@@ -2572,6 +2582,9 @@
       <c r="G89">
         <v>1</v>
       </c>
+      <c r="H89" s="1">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90">
@@ -2592,6 +2605,9 @@
       <c r="G90">
         <v>2</v>
       </c>
+      <c r="H90" s="1">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91">
@@ -2612,6 +2628,9 @@
       <c r="G91">
         <v>3</v>
       </c>
+      <c r="H91" s="1">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92">
@@ -2632,6 +2651,9 @@
       <c r="G92">
         <v>1</v>
       </c>
+      <c r="H92" s="1">
+        <v>10</v>
+      </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93">
@@ -2652,6 +2674,9 @@
       <c r="G93">
         <v>2</v>
       </c>
+      <c r="H93" s="1">
+        <v>10</v>
+      </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94">
@@ -2672,6 +2697,9 @@
       <c r="G94">
         <v>3</v>
       </c>
+      <c r="H94" s="1">
+        <v>10</v>
+      </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95">
@@ -2692,6 +2720,9 @@
       <c r="G95">
         <v>1</v>
       </c>
+      <c r="H95" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A96">
@@ -2712,8 +2743,11 @@
       <c r="G96">
         <v>2</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H96" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>87</v>
       </c>
@@ -2732,8 +2766,11 @@
       <c r="G97">
         <v>3</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H97" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>88</v>
       </c>
@@ -2752,8 +2789,11 @@
       <c r="G98">
         <v>1</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H98" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>89</v>
       </c>
@@ -2772,8 +2812,11 @@
       <c r="G99">
         <v>2</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H99" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>90</v>
       </c>
@@ -2792,8 +2835,11 @@
       <c r="G100">
         <v>3</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H100" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>91</v>
       </c>
@@ -2812,8 +2858,11 @@
       <c r="G101">
         <v>1</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H101" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>92</v>
       </c>
@@ -2832,8 +2881,11 @@
       <c r="G102">
         <v>2</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H102" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>93</v>
       </c>
@@ -2852,8 +2904,11 @@
       <c r="G103">
         <v>3</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H103" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>94</v>
       </c>
@@ -2872,8 +2927,11 @@
       <c r="G104">
         <v>1</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H104" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>95</v>
       </c>
@@ -2892,8 +2950,11 @@
       <c r="G105">
         <v>2</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H105" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>96</v>
       </c>
@@ -2912,8 +2973,11 @@
       <c r="G106">
         <v>3</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H106" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>97</v>
       </c>
@@ -2932,8 +2996,11 @@
       <c r="G107">
         <v>1</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H107" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>98</v>
       </c>
@@ -2952,8 +3019,11 @@
       <c r="G108">
         <v>2</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H108" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>99</v>
       </c>
@@ -2972,8 +3042,11 @@
       <c r="G109">
         <v>3</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H109" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>100</v>
       </c>
@@ -2992,8 +3065,11 @@
       <c r="G110">
         <v>1</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H110" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>101</v>
       </c>
@@ -3012,8 +3088,11 @@
       <c r="G111">
         <v>2</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H111" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>102</v>
       </c>
@@ -3032,8 +3111,11 @@
       <c r="G112">
         <v>3</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H112" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>103</v>
       </c>
@@ -3052,8 +3134,11 @@
       <c r="G113">
         <v>1</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H113" s="1">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>104</v>
       </c>
@@ -3072,8 +3157,11 @@
       <c r="G114">
         <v>2</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H114" s="1">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>105</v>
       </c>
@@ -3092,8 +3180,11 @@
       <c r="G115">
         <v>3</v>
       </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H115" s="1">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>106</v>
       </c>
@@ -3112,8 +3203,11 @@
       <c r="G116">
         <v>1</v>
       </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H116" s="1">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>107</v>
       </c>
@@ -3133,7 +3227,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>108</v>
       </c>
@@ -3153,7 +3247,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>109</v>
       </c>
@@ -3173,7 +3267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>110</v>
       </c>
@@ -3193,7 +3287,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>111</v>
       </c>
@@ -3213,7 +3307,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>112</v>
       </c>
@@ -3233,7 +3327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>113</v>
       </c>
@@ -3253,7 +3347,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>114</v>
       </c>
@@ -3273,7 +3367,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>115</v>
       </c>
@@ -3293,7 +3387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>116</v>
       </c>
@@ -3313,7 +3407,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>117</v>
       </c>
@@ -3333,7 +3427,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>118</v>
       </c>

</xml_diff>

<commit_message>
added new volumes filtered
</commit_message>
<xml_diff>
--- a/data/permanent mount index.xlsx
+++ b/data/permanent mount index.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SFOURNIE\Git\fluoroproj\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{437C1489-2E86-4FDA-8BB3-5F8BCCBBB550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B7CF471-7A5B-404B-B8C2-EA3461F91566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9E43A6A2-D3AC-4401-99CB-597ABF4CC040}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{9E43A6A2-D3AC-4401-99CB-597ABF4CC040}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -466,23 +466,23 @@
   <dimension ref="A1:H145"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H116" sqref="H116"/>
+      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K132" sqref="K132"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -508,7 +508,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -531,7 +531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -554,7 +554,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -577,7 +577,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -600,7 +600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -623,7 +623,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -646,7 +646,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -669,7 +669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -692,7 +692,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -715,7 +715,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -741,7 +741,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2</v>
       </c>
@@ -767,7 +767,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>3</v>
       </c>
@@ -793,7 +793,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>4</v>
       </c>
@@ -819,7 +819,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>5</v>
       </c>
@@ -845,7 +845,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>6</v>
       </c>
@@ -871,7 +871,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>7</v>
       </c>
@@ -897,7 +897,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>8</v>
       </c>
@@ -923,7 +923,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>9</v>
       </c>
@@ -949,7 +949,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>10</v>
       </c>
@@ -975,7 +975,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>11</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>12</v>
       </c>
@@ -1027,7 +1027,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>13</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>14</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>15</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>16</v>
       </c>
@@ -1131,7 +1131,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>17</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>18</v>
       </c>
@@ -1183,7 +1183,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>19</v>
       </c>
@@ -1206,7 +1206,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>20</v>
       </c>
@@ -1229,7 +1229,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>21</v>
       </c>
@@ -1252,7 +1252,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>22</v>
       </c>
@@ -1275,7 +1275,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>23</v>
       </c>
@@ -1298,7 +1298,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>24</v>
       </c>
@@ -1321,7 +1321,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>25</v>
       </c>
@@ -1344,7 +1344,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>26</v>
       </c>
@@ -1367,7 +1367,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>27</v>
       </c>
@@ -1390,7 +1390,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>28</v>
       </c>
@@ -1413,7 +1413,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>29</v>
       </c>
@@ -1436,7 +1436,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>30</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>31</v>
       </c>
@@ -1482,7 +1482,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>32</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>33</v>
       </c>
@@ -1528,7 +1528,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>34</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>35</v>
       </c>
@@ -1574,7 +1574,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>36</v>
       </c>
@@ -1597,7 +1597,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>37</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>38</v>
       </c>
@@ -1643,7 +1643,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>39</v>
       </c>
@@ -1666,7 +1666,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>40</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>41</v>
       </c>
@@ -1712,7 +1712,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>42</v>
       </c>
@@ -1735,7 +1735,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>43</v>
       </c>
@@ -1758,7 +1758,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>44</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>45</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>46</v>
       </c>
@@ -1827,7 +1827,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>47</v>
       </c>
@@ -1850,7 +1850,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>48</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>49</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>50</v>
       </c>
@@ -1919,7 +1919,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>51</v>
       </c>
@@ -1942,7 +1942,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>52</v>
       </c>
@@ -1965,7 +1965,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>53</v>
       </c>
@@ -1988,7 +1988,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>54</v>
       </c>
@@ -2011,7 +2011,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>55</v>
       </c>
@@ -2034,7 +2034,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>56</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>57</v>
       </c>
@@ -2080,7 +2080,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>58</v>
       </c>
@@ -2103,7 +2103,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>59</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>60</v>
       </c>
@@ -2149,7 +2149,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>61</v>
       </c>
@@ -2172,7 +2172,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>62</v>
       </c>
@@ -2195,7 +2195,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>63</v>
       </c>
@@ -2218,7 +2218,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>64</v>
       </c>
@@ -2241,7 +2241,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>65</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>66</v>
       </c>
@@ -2287,7 +2287,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>67</v>
       </c>
@@ -2310,7 +2310,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>68</v>
       </c>
@@ -2333,7 +2333,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>69</v>
       </c>
@@ -2356,7 +2356,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>70</v>
       </c>
@@ -2379,7 +2379,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>71</v>
       </c>
@@ -2402,7 +2402,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>72</v>
       </c>
@@ -2425,7 +2425,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>73</v>
       </c>
@@ -2448,7 +2448,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>74</v>
       </c>
@@ -2471,7 +2471,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>75</v>
       </c>
@@ -2494,7 +2494,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>76</v>
       </c>
@@ -2517,7 +2517,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>77</v>
       </c>
@@ -2540,7 +2540,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>78</v>
       </c>
@@ -2563,7 +2563,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>79</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>80</v>
       </c>
@@ -2609,7 +2609,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>81</v>
       </c>
@@ -2632,7 +2632,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>82</v>
       </c>
@@ -2655,7 +2655,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>83</v>
       </c>
@@ -2678,7 +2678,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>84</v>
       </c>
@@ -2701,7 +2701,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>85</v>
       </c>
@@ -2724,7 +2724,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>86</v>
       </c>
@@ -2747,7 +2747,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>87</v>
       </c>
@@ -2770,7 +2770,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>88</v>
       </c>
@@ -2793,7 +2793,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>89</v>
       </c>
@@ -2816,7 +2816,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>90</v>
       </c>
@@ -2839,7 +2839,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>91</v>
       </c>
@@ -2862,7 +2862,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>92</v>
       </c>
@@ -2885,7 +2885,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>93</v>
       </c>
@@ -2908,7 +2908,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>94</v>
       </c>
@@ -2931,7 +2931,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>95</v>
       </c>
@@ -2954,7 +2954,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>96</v>
       </c>
@@ -2977,7 +2977,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>97</v>
       </c>
@@ -3000,7 +3000,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>98</v>
       </c>
@@ -3023,7 +3023,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>99</v>
       </c>
@@ -3046,7 +3046,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>100</v>
       </c>
@@ -3069,7 +3069,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>101</v>
       </c>
@@ -3092,7 +3092,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>102</v>
       </c>
@@ -3115,7 +3115,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>103</v>
       </c>
@@ -3138,7 +3138,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>104</v>
       </c>
@@ -3161,7 +3161,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>105</v>
       </c>
@@ -3184,7 +3184,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>106</v>
       </c>
@@ -3204,10 +3204,10 @@
         <v>1</v>
       </c>
       <c r="H116" s="1">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>107</v>
       </c>
@@ -3226,8 +3226,11 @@
       <c r="G117">
         <v>2</v>
       </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H117" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>108</v>
       </c>
@@ -3246,8 +3249,11 @@
       <c r="G118">
         <v>3</v>
       </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H118" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>109</v>
       </c>
@@ -3266,8 +3272,11 @@
       <c r="G119">
         <v>1</v>
       </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H119" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>110</v>
       </c>
@@ -3286,8 +3295,11 @@
       <c r="G120">
         <v>2</v>
       </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H120" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>111</v>
       </c>
@@ -3306,8 +3318,11 @@
       <c r="G121">
         <v>3</v>
       </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H121" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>112</v>
       </c>
@@ -3326,8 +3341,11 @@
       <c r="G122">
         <v>1</v>
       </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H122" s="1">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>113</v>
       </c>
@@ -3346,8 +3364,11 @@
       <c r="G123">
         <v>2</v>
       </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H123" s="1">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>114</v>
       </c>
@@ -3366,8 +3387,11 @@
       <c r="G124">
         <v>3</v>
       </c>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H124" s="1">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>115</v>
       </c>
@@ -3386,8 +3410,11 @@
       <c r="G125">
         <v>1</v>
       </c>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H125" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>116</v>
       </c>
@@ -3406,8 +3433,11 @@
       <c r="G126">
         <v>2</v>
       </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H126" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>117</v>
       </c>
@@ -3426,8 +3456,11 @@
       <c r="G127">
         <v>3</v>
       </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H127" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>118</v>
       </c>
@@ -3446,8 +3479,11 @@
       <c r="G128">
         <v>1</v>
       </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H128" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>119</v>
       </c>
@@ -3466,8 +3502,11 @@
       <c r="G129">
         <v>2</v>
       </c>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H129" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>120</v>
       </c>
@@ -3486,8 +3525,11 @@
       <c r="G130">
         <v>3</v>
       </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H130" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>121</v>
       </c>
@@ -3506,8 +3548,11 @@
       <c r="G131">
         <v>1</v>
       </c>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H131" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>122</v>
       </c>
@@ -3526,8 +3571,11 @@
       <c r="G132">
         <v>2</v>
       </c>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H132" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>123</v>
       </c>
@@ -3546,8 +3594,11 @@
       <c r="G133">
         <v>3</v>
       </c>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H133" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>124</v>
       </c>
@@ -3566,8 +3617,11 @@
       <c r="G134">
         <v>1</v>
       </c>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H134" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>125</v>
       </c>
@@ -3586,8 +3640,11 @@
       <c r="G135">
         <v>2</v>
       </c>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H135" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>126</v>
       </c>
@@ -3606,8 +3663,11 @@
       <c r="G136">
         <v>3</v>
       </c>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H136" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>127</v>
       </c>
@@ -3626,8 +3686,11 @@
       <c r="G137">
         <v>1</v>
       </c>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H137" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>128</v>
       </c>
@@ -3646,8 +3709,11 @@
       <c r="G138">
         <v>2</v>
       </c>
-    </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H138" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>129</v>
       </c>
@@ -3666,8 +3732,11 @@
       <c r="G139">
         <v>3</v>
       </c>
-    </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H139" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>130</v>
       </c>
@@ -3686,8 +3755,11 @@
       <c r="G140">
         <v>1</v>
       </c>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H140" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>131</v>
       </c>
@@ -3706,8 +3778,11 @@
       <c r="G141">
         <v>2</v>
       </c>
-    </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H141" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>132</v>
       </c>
@@ -3726,8 +3801,11 @@
       <c r="G142">
         <v>3</v>
       </c>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H142" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>133</v>
       </c>
@@ -3746,8 +3824,11 @@
       <c r="G143">
         <v>1</v>
       </c>
-    </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H143" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>134</v>
       </c>
@@ -3766,8 +3847,11 @@
       <c r="G144">
         <v>2</v>
       </c>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H144" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>135</v>
       </c>
@@ -3785,6 +3869,9 @@
       </c>
       <c r="G145">
         <v>3</v>
+      </c>
+      <c r="H145" s="1">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>